<commit_message>
after adding the new chrome driver
</commit_message>
<xml_diff>
--- a/TestData/FlightSearch.xlsx
+++ b/TestData/FlightSearch.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67474F-A62E-4555-9C44-195AB70F143B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4751501-1917-42C4-B020-58F5E355388C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Origin</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>Madrid</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Brisbane</t>
   </si>
 </sst>
 </file>
@@ -349,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -373,6 +385,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>